<commit_message>
Inserir tabela modelo B3
</commit_message>
<xml_diff>
--- a/Operacao.xlsx
+++ b/Operacao.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/18730566c04dc4cc/PC - Pessoal/01 - Controle pessoal/Contas banco/0-planilha Patrick/Python - alfa/my_app_API/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/18730566c04dc4cc/PC - Pessoal/01 - Controle pessoal/Contas banco/0-planilha Patrick/App-streamlit-front/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="13_ncr:1_{6C7302AE-98AF-4145-937B-F223C186D0F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5656971B-A003-45D2-8E9F-9E7BBE186A37}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="13_ncr:1_{6C7302AE-98AF-4145-937B-F223C186D0F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8191F9C7-006C-41F0-B779-2687EB1D2EAB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FECB4E4C-02E1-4AF1-90C3-3A9A55626EBA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FECB4E4C-02E1-4AF1-90C3-3A9A55626EBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha3" sheetId="3" r:id="rId2"/>
-    <sheet name="Planilha2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$I$1694</definedName>
@@ -41,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>Ações</t>
   </si>
@@ -136,17 +134,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -162,10 +155,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -531,106 +520,106 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="1">
         <v>44014</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2">
         <v>26</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2">
         <v>643.96</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2">
         <v>0.2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="1">
         <v>43977</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3">
         <v>4</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3">
         <v>74.819999999999993</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3">
         <v>0.02</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="1">
         <v>43976</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4">
         <v>6</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4">
         <v>148.91</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4">
         <v>0.05</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="1">
         <v>44482</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5">
         <v>45</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5">
         <v>1057.82</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5">
         <v>0.32</v>
       </c>
     </row>
@@ -774,7 +763,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
-      <c r="I52" s="3"/>
+      <c r="I52" s="2"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
@@ -790,87 +779,87 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
-      <c r="I57" s="3"/>
+      <c r="I57" s="2"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
-      <c r="I58" s="3"/>
+      <c r="I58" s="2"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
-      <c r="I59" s="3"/>
+      <c r="I59" s="2"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
-      <c r="I60" s="3"/>
+      <c r="I60" s="2"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
-      <c r="I61" s="3"/>
+      <c r="I61" s="2"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
-      <c r="I62" s="3"/>
+      <c r="I62" s="2"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
-      <c r="I63" s="3"/>
+      <c r="I63" s="2"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
-      <c r="I64" s="3"/>
+      <c r="I64" s="2"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
-      <c r="I65" s="3"/>
+      <c r="I65" s="2"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
-      <c r="I66" s="3"/>
+      <c r="I66" s="2"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
-      <c r="I67" s="3"/>
+      <c r="I67" s="2"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
-      <c r="I68" s="3"/>
+      <c r="I68" s="2"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
-      <c r="I69" s="3"/>
+      <c r="I69" s="2"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
-      <c r="I70" s="4"/>
+      <c r="I70" s="3"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
-      <c r="I71" s="3"/>
+      <c r="I71" s="2"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
-      <c r="I72" s="3"/>
+      <c r="I72" s="2"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
-      <c r="I73" s="3"/>
+      <c r="I73" s="2"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
-      <c r="I74" s="3"/>
+      <c r="I74" s="2"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
-      <c r="I75" s="3"/>
+      <c r="I75" s="2"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
-      <c r="I76" s="3"/>
+      <c r="I76" s="2"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
-      <c r="I77" s="5"/>
+      <c r="I77" s="4"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
@@ -5736,144 +5725,4 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{683FF497-5E80-47FE-A4C3-557A43E68936}">
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="A1:H4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>44014</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1">
-        <v>26</v>
-      </c>
-      <c r="F1">
-        <v>643.96</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>43977</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2">
-        <v>74.819999999999993</v>
-      </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>43976</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
-      <c r="F3">
-        <v>148.91</v>
-      </c>
-      <c r="G3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>44482</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>45</v>
-      </c>
-      <c r="F4">
-        <v>1057.82</v>
-      </c>
-      <c r="G4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>0.32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CBCB4D9-A0E6-4AD6-A494-F4C4D4F996A1}">
-  <dimension ref="B2"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="175.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>